<commit_message>
Info Folder Formatting Adjustments
Removed marinefrigate file, no changes from v2.1
Nerfed light corvs vs colls a bit more.
Info Folder Formatting Adjustments
</commit_message>
<xml_diff>
--- a/BalanceInfo/2.3 Players Patch - Balance Design.xlsx
+++ b/BalanceInfo/2.3 Players Patch - Balance Design.xlsx
@@ -1985,7 +1985,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2020,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="36">
-        <v>43312</v>
+        <v>43314</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>6</v>

</xml_diff>